<commit_message>
Better UAC flags handling added
</commit_message>
<xml_diff>
--- a/GetADobjects/AD Column map.xlsx
+++ b/GetADobjects/AD Column map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" tabRatio="625"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20760" windowHeight="8700" tabRatio="625"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="9" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Computers!$A$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Contacts!$A$1:$I$58</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Groups!$A$1:$I$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Users!$A$1:$I$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Users!$A$1:$I$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WellKnownSIDs!$A$1:$I$8</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="182">
   <si>
     <t>max_length</t>
   </si>
@@ -569,6 +569,18 @@
   </si>
   <si>
     <t>PostOp</t>
+  </si>
+  <si>
+    <t>PasswordExpiryTime</t>
+  </si>
+  <si>
+    <t>msDS-UserPasswordExpiryTimeComputed</t>
+  </si>
+  <si>
+    <t>ManagerGUID</t>
+  </si>
+  <si>
+    <t>:: NOT Populated by CLR SP ::</t>
   </si>
 </sst>
 </file>
@@ -904,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H67"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,7 +991,7 @@
         <v>new TableColDef("GivenName", typeof(String), "givenname","Adprop"),</v>
       </c>
       <c r="I2" t="str">
-        <f>CONCATENATE("[",C2,"] [",A2,"](",D2,") ",E2,",")</f>
+        <f t="shared" ref="I2:I27" si="0">CONCATENATE("[",C2,"] [",A2,"](",D2,") ",E2,",")</f>
         <v>[GivenName] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -1006,11 +1018,11 @@
         <v>156</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H66" si="0">CONCATENATE("new TableColDef(""",C3,""", typeof(",B3,"), """,G3,""",""",F3,"""),")</f>
+        <f t="shared" ref="H3:H67" si="1">CONCATENATE("new TableColDef(""",C3,""", typeof(",B3,"), """,G3,""",""",F3,"""),")</f>
         <v>new TableColDef("Initials", typeof(String), "initials","Adprop"),</v>
       </c>
       <c r="I3" t="str">
-        <f>CONCATENATE("[",C3,"] [",A3,"](",D3,") ",E3,",")</f>
+        <f t="shared" si="0"/>
         <v>[Initials] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -1037,11 +1049,11 @@
         <v>103</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Surname", typeof(String), "sn","Adprop"),</v>
       </c>
       <c r="I4" t="str">
-        <f>CONCATENATE("[",C4,"] [",A4,"](",D4,") ",E4,",")</f>
+        <f t="shared" si="0"/>
         <v>[Surname] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -1068,11 +1080,11 @@
         <v>115</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("DisplayName", typeof(String), "displayname","Adprop"),</v>
       </c>
       <c r="I5" t="str">
-        <f>CONCATENATE("[",C5,"] [",A5,"](",D5,") ",E5,",")</f>
+        <f t="shared" si="0"/>
         <v>[DisplayName] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -1099,11 +1111,11 @@
         <v>101</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Description", typeof(String), "description","Adprop"),</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("[",C6,"] [",A6,"](",D6,") ",E6,",")</f>
+        <f t="shared" si="0"/>
         <v>[Description] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -1130,11 +1142,11 @@
         <v>79</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Office", typeof(String), "physicalDeliveryOfficeName","Adprop"),</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE("[",C7,"] [",A7,"](",D7,") ",E7,",")</f>
+        <f t="shared" si="0"/>
         <v>[Office] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -1161,11 +1173,11 @@
         <v>155</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("OfficePhone", typeof(String), "telephonenumber","Adprop"),</v>
       </c>
       <c r="I8" t="str">
-        <f>CONCATENATE("[",C8,"] [",A8,"](",D8,") ",E8,",")</f>
+        <f t="shared" si="0"/>
         <v>[OfficePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -1192,11 +1204,11 @@
         <v>102</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("EmailAddress", typeof(String), "mail","Adprop"),</v>
       </c>
       <c r="I9" t="str">
-        <f>CONCATENATE("[",C9,"] [",A9,"](",D9,") ",E9,",")</f>
+        <f t="shared" si="0"/>
         <v>[EmailAddress] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -1223,11 +1235,11 @@
         <v>165</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("HomePage", typeof(String), "wwwhomepage","Adprop"),</v>
       </c>
       <c r="I10" t="str">
-        <f>CONCATENATE("[",C10,"] [",A10,"](",D10,") ",E10,",")</f>
+        <f t="shared" si="0"/>
         <v>[HomePage] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -1254,11 +1266,11 @@
         <v>171</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("StreetAddress", typeof(String), "streetaddress","Adprop"),</v>
       </c>
       <c r="I11" t="str">
-        <f>CONCATENATE("[",C11,"] [",A11,"](",D11,") ",E11,",")</f>
+        <f t="shared" si="0"/>
         <v>[StreetAddress] [nvarchar](160) NULL,</v>
       </c>
     </row>
@@ -1285,11 +1297,11 @@
         <v>167</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("POBox", typeof(String), "postofficebox","Adprop"),</v>
       </c>
       <c r="I12" t="str">
-        <f>CONCATENATE("[",C12,"] [",A12,"](",D12,") ",E12,",")</f>
+        <f t="shared" si="0"/>
         <v>[POBox] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -1316,11 +1328,11 @@
         <v>83</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("City", typeof(String), "l","Adprop"),</v>
       </c>
       <c r="I13" t="str">
-        <f>CONCATENATE("[",C13,"] [",A13,"](",D13,") ",E13,",")</f>
+        <f t="shared" si="0"/>
         <v>[City] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -1347,11 +1359,11 @@
         <v>78</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("State", typeof(String), "st","Adprop"),</v>
       </c>
       <c r="I14" t="str">
-        <f>CONCATENATE("[",C14,"] [",A14,"](",D14,") ",E14,",")</f>
+        <f t="shared" si="0"/>
         <v>[State] [nvarchar](64) NULL,</v>
       </c>
     </row>
@@ -1378,11 +1390,11 @@
         <v>168</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("PostalCode", typeof(String), "postalcode","Adprop"),</v>
       </c>
       <c r="I15" t="str">
-        <f>CONCATENATE("[",C15,"] [",A15,"](",D15,") ",E15,",")</f>
+        <f t="shared" si="0"/>
         <v>[PostalCode] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -1409,11 +1421,11 @@
         <v>77</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Country", typeof(String), "co","Adprop"),</v>
       </c>
       <c r="I16" t="str">
-        <f>CONCATENATE("[",C16,"] [",A16,"](",D16,") ",E16,",")</f>
+        <f t="shared" si="0"/>
         <v>[Country] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -1440,11 +1452,11 @@
         <v>160</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("HomePhone", typeof(String), "homephone","Adprop"),</v>
       </c>
       <c r="I17" t="str">
-        <f>CONCATENATE("[",C17,"] [",A17,"](",D17,") ",E17,",")</f>
+        <f t="shared" si="0"/>
         <v>[HomePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -1471,11 +1483,11 @@
         <v>166</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Pager", typeof(String), "pager","Adprop"),</v>
       </c>
       <c r="I18" t="str">
-        <f>CONCATENATE("[",C18,"] [",A18,"](",D18,") ",E18,",")</f>
+        <f t="shared" si="0"/>
         <v>[Pager] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -1502,11 +1514,11 @@
         <v>82</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("MobilePhone", typeof(String), "mobile","Adprop"),</v>
       </c>
       <c r="I19" t="str">
-        <f>CONCATENATE("[",C19,"] [",A19,"](",D19,") ",E19,",")</f>
+        <f t="shared" si="0"/>
         <v>[MobilePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -1533,11 +1545,11 @@
         <v>84</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Fax", typeof(String), "facsimileTelephoneNumber","Adprop"),</v>
       </c>
       <c r="I20" t="str">
-        <f>CONCATENATE("[",C20,"] [",A20,"](",D20,") ",E20,",")</f>
+        <f t="shared" si="0"/>
         <v>[Fax] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -1564,11 +1576,11 @@
         <v>149</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Title", typeof(String), "title","Adprop"),</v>
       </c>
       <c r="I21" t="str">
-        <f>CONCATENATE("[",C21,"] [",A21,"](",D21,") ",E21,",")</f>
+        <f t="shared" si="0"/>
         <v>[Title] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -1595,11 +1607,11 @@
         <v>159</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Department", typeof(String), "department","Adprop"),</v>
       </c>
       <c r="I22" t="str">
-        <f>CONCATENATE("[",C22,"] [",A22,"](",D22,") ",E22,",")</f>
+        <f t="shared" si="0"/>
         <v>[Department] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -1626,11 +1638,11 @@
         <v>154</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Company", typeof(String), "company","Adprop"),</v>
       </c>
       <c r="I23" t="str">
-        <f>CONCATENATE("[",C23,"] [",A23,"](",D23,") ",E23,",")</f>
+        <f t="shared" si="0"/>
         <v>[Company] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -1657,11 +1669,11 @@
         <v>158</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Manager", typeof(String), "manager","Adprop"),</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE("[",C24,"] [",A24,"](",D24,") ",E24,",")</f>
+        <f t="shared" si="0"/>
         <v>[Manager] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -1688,11 +1700,11 @@
         <v>152</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("EmployeeID", typeof(String), "employeeid","Adprop"),</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE("[",C25,"] [",A25,"](",D25,") ",E25,",")</f>
+        <f t="shared" si="0"/>
         <v>[EmployeeID] [nvarchar](64) NULL,</v>
       </c>
     </row>
@@ -1719,11 +1731,11 @@
         <v>162</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("EmployeeNumber", typeof(String), "employeenumber","Adprop"),</v>
       </c>
       <c r="I26" t="str">
-        <f>CONCATENATE("[",C26,"] [",A26,"](",D26,") ",E26,",")</f>
+        <f t="shared" si="0"/>
         <v>[EmployeeNumber] [nvarchar](64) NULL,</v>
       </c>
     </row>
@@ -1750,11 +1762,11 @@
         <v>161</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Division", typeof(String), "division","Adprop"),</v>
       </c>
       <c r="I27" t="str">
-        <f>CONCATENATE("[",C27,"] [",A27,"](",D27,") ",E27,",")</f>
+        <f t="shared" si="0"/>
         <v>[Division] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -1778,11 +1790,11 @@
         <v>135</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Enabled", typeof(Boolean), "ACCOUNTDISABLE","UAC"),</v>
       </c>
       <c r="I28" t="str">
-        <f>CONCATENATE("[",C28,"] [",A28,"] ",E28,",")</f>
+        <f t="shared" ref="I28:I50" si="2">CONCATENATE("[",C28,"] [",A28,"] ",E28,",")</f>
         <v>[Enabled] [bit] NULL,</v>
       </c>
     </row>
@@ -1806,11 +1818,11 @@
         <v>140</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("LockedOut", typeof(Boolean), "LOCKOUT","UAC"),</v>
       </c>
       <c r="I29" t="str">
-        <f>CONCATENATE("[",C29,"] [",A29,"] ",E29,",")</f>
+        <f t="shared" si="2"/>
         <v>[LockedOut] [bit] NULL,</v>
       </c>
     </row>
@@ -1834,11 +1846,11 @@
         <v>89</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("MNSLogonAccount", typeof(Boolean), "MNS_LOGON_ACCOUNT","UAC"),</v>
       </c>
       <c r="I30" t="str">
-        <f>CONCATENATE("[",C30,"] [",A30,"] ",E30,",")</f>
+        <f t="shared" si="2"/>
         <v>[MNSLogonAccount] [bit] NULL,</v>
       </c>
     </row>
@@ -1862,11 +1874,11 @@
         <v>137</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("CannotChangePassword", typeof(Boolean), "PASSWD_CANT_CHANGE","UAC"),</v>
       </c>
       <c r="I31" t="str">
-        <f>CONCATENATE("[",C31,"] [",A31,"] ",E31,",")</f>
+        <f t="shared" si="2"/>
         <v>[CannotChangePassword] [bit] NULL,</v>
       </c>
     </row>
@@ -1890,11 +1902,11 @@
         <v>90</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("PasswordExpired", typeof(Boolean), "PASSWORD_EXPIRED","UAC"),</v>
       </c>
       <c r="I32" t="str">
-        <f>CONCATENATE("[",C32,"] [",A32,"] ",E32,",")</f>
+        <f t="shared" si="2"/>
         <v>[PasswordExpired] [bit] NULL,</v>
       </c>
     </row>
@@ -1918,11 +1930,11 @@
         <v>138</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("PasswordNeverExpires", typeof(Boolean), "DONT_EXPIRE_PASSWD","UAC"),</v>
       </c>
       <c r="I33" t="str">
-        <f>CONCATENATE("[",C33,"] [",A33,"] ",E33,",")</f>
+        <f t="shared" si="2"/>
         <v>[PasswordNeverExpires] [bit] NULL,</v>
       </c>
     </row>
@@ -1946,11 +1958,11 @@
         <v>136</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("PasswordNotRequired", typeof(Boolean), "PASSWD_NOTREQD","UAC"),</v>
       </c>
       <c r="I34" t="str">
-        <f>CONCATENATE("[",C34,"] [",A34,"] ",E34,",")</f>
+        <f t="shared" si="2"/>
         <v>[PasswordNotRequired] [bit] NULL,</v>
       </c>
     </row>
@@ -1974,11 +1986,11 @@
         <v>139</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("SmartcardLogonRequired", typeof(Boolean), "SMARTCARD_REQUIRED","UAC"),</v>
       </c>
       <c r="I35" t="str">
-        <f>CONCATENATE("[",C35,"] [",A35,"] ",E35,",")</f>
+        <f t="shared" si="2"/>
         <v>[SmartcardLogonRequired] [bit] NULL,</v>
       </c>
     </row>
@@ -2002,11 +2014,11 @@
         <v>93</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("DoesNotRequirePreAuth", typeof(Boolean), "DONT_REQ_PREAUTH","UAC"),</v>
       </c>
       <c r="I36" t="str">
-        <f>CONCATENATE("[",C36,"] [",A36,"] ",E36,",")</f>
+        <f t="shared" si="2"/>
         <v>[DoesNotRequirePreAuth] [bit] NULL,</v>
       </c>
     </row>
@@ -2030,11 +2042,11 @@
         <v>141</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("AllowReversiblePasswordEncryption", typeof(Boolean), "ENCRYPTED_TEXT_PWD_ALLOWED","UAC"),</v>
       </c>
       <c r="I37" t="str">
-        <f>CONCATENATE("[",C37,"] [",A37,"] ",E37,",")</f>
+        <f t="shared" si="2"/>
         <v>[AllowReversiblePasswordEncryption] [bit] NULL,</v>
       </c>
     </row>
@@ -2058,11 +2070,11 @@
         <v>91</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("AccountNotDelegated", typeof(Boolean), "NOT_DELEGATED","UAC"),</v>
       </c>
       <c r="I38" t="str">
-        <f>CONCATENATE("[",C38,"] [",A38,"] ",E38,",")</f>
+        <f t="shared" si="2"/>
         <v>[AccountNotDelegated] [bit] NULL,</v>
       </c>
     </row>
@@ -2086,11 +2098,11 @@
         <v>88</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("TrustedForDelegation", typeof(Boolean), "TRUSTED_FOR_DELEGATION","UAC"),</v>
       </c>
       <c r="I39" t="str">
-        <f>CONCATENATE("[",C39,"] [",A39,"] ",E39,",")</f>
+        <f t="shared" si="2"/>
         <v>[TrustedForDelegation] [bit] NULL,</v>
       </c>
     </row>
@@ -2114,11 +2126,11 @@
         <v>86</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("TrustedToAuthForDelegation", typeof(Boolean), "TRUSTED_TO_AUTH_FOR_DELEGATION","UAC"),</v>
       </c>
       <c r="I40" t="str">
-        <f>CONCATENATE("[",C40,"] [",A40,"] ",E40,",")</f>
+        <f t="shared" si="2"/>
         <v>[TrustedToAuthForDelegation] [bit] NULL,</v>
       </c>
     </row>
@@ -2142,11 +2154,11 @@
         <v>87</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("UseDESKeyOnly", typeof(Boolean), "USE_DES_KEY_ONLY","UAC"),</v>
       </c>
       <c r="I41" t="str">
-        <f>CONCATENATE("[",C41,"] [",A41,"] ",E41,",")</f>
+        <f t="shared" si="2"/>
         <v>[UseDESKeyOnly] [bit] NULL,</v>
       </c>
     </row>
@@ -2170,11 +2182,11 @@
         <v>92</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("HomedirRequired", typeof(Boolean), "HOMEDIR_REQUIRED","UAC"),</v>
       </c>
       <c r="I42" t="str">
-        <f>CONCATENATE("[",C42,"] [",A42,"] ",E42,",")</f>
+        <f t="shared" si="2"/>
         <v>[HomedirRequired] [bit] NULL,</v>
       </c>
     </row>
@@ -2198,11 +2210,11 @@
         <v>130</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("LastBadPasswordAttempt", typeof(DateTime), "badpasswordtime","filetime"),</v>
       </c>
       <c r="I43" t="str">
-        <f>CONCATENATE("[",C43,"] [",A43,"] ",E43,",")</f>
+        <f t="shared" si="2"/>
         <v>[LastBadPasswordAttempt] [datetime] NULL,</v>
       </c>
     </row>
@@ -2226,11 +2238,11 @@
         <v>124</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("BadLogonCount", typeof(Int32), "badpwdcount","Adprop"),</v>
       </c>
       <c r="I44" t="str">
-        <f>CONCATENATE("[",C44,"] [",A44,"] ",E44,",")</f>
+        <f t="shared" si="2"/>
         <v>[BadLogonCount] [int] NULL,</v>
       </c>
     </row>
@@ -2254,11 +2266,11 @@
         <v>173</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("LastLogonDate", typeof(DateTime), "lastlogon","filetime"),</v>
       </c>
       <c r="I45" t="str">
-        <f>CONCATENATE("[",C45,"] [",A45,"] ",E45,",")</f>
+        <f t="shared" si="2"/>
         <v>[LastLogonDate] [datetime] NULL,</v>
       </c>
     </row>
@@ -2282,11 +2294,11 @@
         <v>121</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("LogonCount", typeof(Int32), "logoncount","Adprop"),</v>
       </c>
       <c r="I46" t="str">
-        <f>CONCATENATE("[",C46,"] [",A46,"] ",E46,",")</f>
+        <f t="shared" si="2"/>
         <v>[LogonCount] [int] NULL,</v>
       </c>
     </row>
@@ -2310,11 +2322,11 @@
         <v>123</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("PasswordLastSet", typeof(DateTime), "pwdlastset","filetime"),</v>
       </c>
       <c r="I47" t="str">
-        <f>CONCATENATE("[",C47,"] [",A47,"] ",E47,",")</f>
+        <f t="shared" si="2"/>
         <v>[PasswordLastSet] [datetime] NULL,</v>
       </c>
     </row>
@@ -2326,7 +2338,7 @@
         <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>178</v>
       </c>
       <c r="E48" t="s">
         <v>96</v>
@@ -2335,15 +2347,15 @@
         <v>144</v>
       </c>
       <c r="G48" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("AccountLockoutTime", typeof(DateTime), "lockouttime","filetime"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("PasswordExpiryTime", typeof(DateTime), "msDS-UserPasswordExpiryTimeComputed","filetime"),</v>
       </c>
       <c r="I48" t="str">
-        <f>CONCATENATE("[",C48,"] [",A48,"] ",E48,",")</f>
-        <v>[AccountLockoutTime] [datetime] NULL,</v>
+        <f t="shared" si="2"/>
+        <v>[PasswordExpiryTime] [datetime] NULL,</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2354,7 +2366,7 @@
         <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E49" t="s">
         <v>96</v>
@@ -2363,46 +2375,43 @@
         <v>144</v>
       </c>
       <c r="G49" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("AccountExpirationDate", typeof(DateTime), "accountexpires","filetime"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("AccountLockoutTime", typeof(DateTime), "lockouttime","filetime"),</v>
       </c>
       <c r="I49" t="str">
-        <f>CONCATENATE("[",C49,"] [",A49,"] ",E49,",")</f>
-        <v>[AccountExpirationDate] [datetime] NULL,</v>
+        <f t="shared" si="2"/>
+        <v>[AccountLockoutTime] [datetime] NULL,</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>75</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50">
-        <v>128</v>
+        <v>73</v>
+      </c>
+      <c r="C50" t="s">
+        <v>3</v>
       </c>
       <c r="E50" t="s">
         <v>96</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G50" t="s">
-        <v>172</v>
+        <v>119</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("LogonWorkstations", typeof(String), "userworkstations","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("AccountExpirationDate", typeof(DateTime), "accountexpires","filetime"),</v>
       </c>
       <c r="I50" t="str">
-        <f>CONCATENATE("[",C50,"] [",A50,"](",D50,") ",E50,",")</f>
-        <v>[LogonWorkstations] [nvarchar](128) NULL,</v>
+        <f t="shared" si="2"/>
+        <v>[AccountExpirationDate] [datetime] NULL,</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2413,7 +2422,7 @@
         <v>75</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D51">
         <v>128</v>
@@ -2425,15 +2434,15 @@
         <v>147</v>
       </c>
       <c r="G51" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("HomeDirectory", typeof(String), "homedirectory","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("LogonWorkstations", typeof(String), "userworkstations","Adprop"),</v>
       </c>
       <c r="I51" t="str">
         <f>CONCATENATE("[",C51,"] [",A51,"](",D51,") ",E51,",")</f>
-        <v>[HomeDirectory] [nvarchar](128) NULL,</v>
+        <v>[LogonWorkstations] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2444,10 +2453,10 @@
         <v>75</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D52">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="E52" t="s">
         <v>96</v>
@@ -2456,15 +2465,15 @@
         <v>147</v>
       </c>
       <c r="G52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("HomeDrive", typeof(String), "homedrive","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("HomeDirectory", typeof(String), "homedirectory","Adprop"),</v>
       </c>
       <c r="I52" t="str">
         <f>CONCATENATE("[",C52,"] [",A52,"](",D52,") ",E52,",")</f>
-        <v>[HomeDrive] [nvarchar](64) NULL,</v>
+        <v>[HomeDirectory] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2474,11 +2483,11 @@
       <c r="B53" t="s">
         <v>75</v>
       </c>
-      <c r="C53" t="s">
-        <v>56</v>
+      <c r="C53" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="D53">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="E53" t="s">
         <v>96</v>
@@ -2487,15 +2496,15 @@
         <v>147</v>
       </c>
       <c r="G53" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H53" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("ProfilePath", typeof(String), "profilepath","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("HomeDrive", typeof(String), "homedrive","Adprop"),</v>
       </c>
       <c r="I53" t="str">
         <f>CONCATENATE("[",C53,"] [",A53,"](",D53,") ",E53,",")</f>
-        <v>[ProfilePath] [nvarchar](128) NULL,</v>
+        <v>[HomeDrive] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2506,10 +2515,10 @@
         <v>75</v>
       </c>
       <c r="C54" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D54">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E54" t="s">
         <v>96</v>
@@ -2518,26 +2527,29 @@
         <v>147</v>
       </c>
       <c r="G54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("ScriptPath", typeof(String), "scriptpath","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("ProfilePath", typeof(String), "profilepath","Adprop"),</v>
       </c>
       <c r="I54" t="str">
         <f>CONCATENATE("[",C54,"] [",A54,"](",D54,") ",E54,",")</f>
-        <v>[ScriptPath] [nvarchar](256) NULL,</v>
+        <v>[ProfilePath] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>85</v>
+        <v>58</v>
+      </c>
+      <c r="D55">
+        <v>256</v>
       </c>
       <c r="E55" t="s">
         <v>96</v>
@@ -2546,15 +2558,15 @@
         <v>147</v>
       </c>
       <c r="G55" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("userAccountControl", typeof(Int32), "useraccountcontrol","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("ScriptPath", typeof(String), "scriptpath","Adprop"),</v>
       </c>
       <c r="I55" t="str">
-        <f>CONCATENATE("[",C55,"] [",A55,"] ",E55,",")</f>
-        <v>[userAccountControl] [int] NULL,</v>
+        <f>CONCATENATE("[",C55,"] [",A55,"](",D55,") ",E55,",")</f>
+        <v>[ScriptPath] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2564,11 +2576,8 @@
       <c r="B56" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D56">
-        <v>128</v>
+      <c r="C56" t="s">
+        <v>85</v>
       </c>
       <c r="E56" t="s">
         <v>96</v>
@@ -2577,29 +2586,29 @@
         <v>147</v>
       </c>
       <c r="G56" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("PrimaryGroupID", typeof(Int32), "primarygroupid","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("userAccountControl", typeof(Int32), "useraccountcontrol","Adprop"),</v>
       </c>
       <c r="I56" t="str">
         <f>CONCATENATE("[",C56,"] [",A56,"] ",E56,",")</f>
-        <v>[PrimaryGroupID] [int] NULL,</v>
+        <v>[userAccountControl] [int] NULL,</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
-      </c>
-      <c r="C57" t="s">
-        <v>43</v>
+        <v>74</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="D57">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E57" t="s">
         <v>96</v>
@@ -2608,15 +2617,15 @@
         <v>147</v>
       </c>
       <c r="G57" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("Name", typeof(String), "name","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("PrimaryGroupID", typeof(Int32), "primarygroupid","Adprop"),</v>
       </c>
       <c r="I57" t="str">
-        <f>CONCATENATE("[",C57,"] [",A57,"](",D57,") ",E57,",")</f>
-        <v>[Name] [nvarchar](256) NULL,</v>
+        <f>CONCATENATE("[",C57,"] [",A57,"] ",E57,",")</f>
+        <v>[PrimaryGroupID] [int] NULL,</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2627,7 +2636,7 @@
         <v>75</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D58">
         <v>256</v>
@@ -2639,15 +2648,15 @@
         <v>147</v>
       </c>
       <c r="G58" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("CN", typeof(String), "cn","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("Name", typeof(String), "name","Adprop"),</v>
       </c>
       <c r="I58" t="str">
         <f>CONCATENATE("[",C58,"] [",A58,"](",D58,") ",E58,",")</f>
-        <v>[CN] [nvarchar](256) NULL,</v>
+        <v>[Name] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2658,7 +2667,7 @@
         <v>75</v>
       </c>
       <c r="C59" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="D59">
         <v>256</v>
@@ -2670,15 +2679,15 @@
         <v>147</v>
       </c>
       <c r="G59" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("UserPrincipalName", typeof(String), "userprincipalname","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("CN", typeof(String), "cn","Adprop"),</v>
       </c>
       <c r="I59" t="str">
         <f>CONCATENATE("[",C59,"] [",A59,"](",D59,") ",E59,",")</f>
-        <v>[UserPrincipalName] [nvarchar](256) NULL,</v>
+        <v>[CN] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2689,10 +2698,10 @@
         <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D60">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="E60" t="s">
         <v>96</v>
@@ -2701,15 +2710,15 @@
         <v>147</v>
       </c>
       <c r="G60" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("SamAccountName", typeof(String), "samaccountname","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("UserPrincipalName", typeof(String), "userprincipalname","Adprop"),</v>
       </c>
       <c r="I60" t="str">
         <f>CONCATENATE("[",C60,"] [",A60,"](",D60,") ",E60,",")</f>
-        <v>[SamAccountName] [nvarchar](128) NULL,</v>
+        <v>[UserPrincipalName] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2720,10 +2729,10 @@
         <v>75</v>
       </c>
       <c r="C61" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="D61">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="E61" t="s">
         <v>96</v>
@@ -2732,26 +2741,29 @@
         <v>147</v>
       </c>
       <c r="G61" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H61" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("DistinguishedName", typeof(String), "distinguishedname","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("SamAccountName", typeof(String), "samaccountname","Adprop"),</v>
       </c>
       <c r="I61" t="str">
         <f>CONCATENATE("[",C61,"] [",A61,"](",D61,") ",E61,",")</f>
-        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
+        <v>[SamAccountName] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>16</v>
+        <v>75</v>
+      </c>
+      <c r="C62" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62">
+        <v>512</v>
       </c>
       <c r="E62" t="s">
         <v>96</v>
@@ -2760,15 +2772,15 @@
         <v>147</v>
       </c>
       <c r="G62" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("Created", typeof(DateTime), "whencreated","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("DistinguishedName", typeof(String), "distinguishedname","Adprop"),</v>
       </c>
       <c r="I62" t="str">
-        <f>CONCATENATE("[",C62,"] [",A62,"] ",E62,",")</f>
-        <v>[Created] [datetime] NULL,</v>
+        <f>CONCATENATE("[",C62,"] [",A62,"](",D62,") ",E62,",")</f>
+        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2779,7 +2791,7 @@
         <v>73</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="E63" t="s">
         <v>96</v>
@@ -2788,29 +2800,26 @@
         <v>147</v>
       </c>
       <c r="G63" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("Modified", typeof(DateTime), "whenchanged","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("Created", typeof(DateTime), "whencreated","Adprop"),</v>
       </c>
       <c r="I63" t="str">
         <f>CONCATENATE("[",C63,"] [",A63,"] ",E63,",")</f>
-        <v>[Modified] [datetime] NULL,</v>
+        <v>[Created] [datetime] NULL,</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
-      </c>
-      <c r="C64" t="s">
-        <v>44</v>
-      </c>
-      <c r="D64">
-        <v>128</v>
+        <v>73</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="E64" t="s">
         <v>96</v>
@@ -2819,15 +2828,15 @@
         <v>147</v>
       </c>
       <c r="G64" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("ObjectCategory", typeof(String), "objectcategory","Adprop"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("Modified", typeof(DateTime), "whenchanged","Adprop"),</v>
       </c>
       <c r="I64" t="str">
-        <f>CONCATENATE("[",C64,"] [",A64,"](",D64,") ",E64,",")</f>
-        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
+        <f>CONCATENATE("[",C64,"] [",A64,"] ",E64,",")</f>
+        <v>[Modified] [datetime] NULL,</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2838,27 +2847,27 @@
         <v>75</v>
       </c>
       <c r="C65" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D65">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="E65" t="s">
         <v>96</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G65" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H65" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("ObjectClass", typeof(String), "SchemaClassName","ObjClass"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("ObjectCategory", typeof(String), "objectcategory","Adprop"),</v>
       </c>
       <c r="I65" t="str">
         <f>CONCATENATE("[",C65,"] [",A65,"](",D65,") ",E65,",")</f>
-        <v>[ObjectClass] [nvarchar](64) NULL,</v>
+        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2869,59 +2878,112 @@
         <v>75</v>
       </c>
       <c r="C66" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D66">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="E66" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>59</v>
+        <v>145</v>
       </c>
       <c r="G66" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>new TableColDef("SID", typeof(String), "objectsid","SID"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("ObjectClass", typeof(String), "SchemaClassName","ObjClass"),</v>
       </c>
       <c r="I66" t="str">
         <f>CONCATENATE("[",C66,"] [",A66,"](",D66,") ",E66,",")</f>
-        <v>[SID] [nvarchar](128) NOT NULL,</v>
+        <v>[ObjectClass] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C67" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="D67">
+        <v>128</v>
       </c>
       <c r="E67" t="s">
         <v>97</v>
       </c>
       <c r="F67" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G67" t="s">
+        <v>112</v>
+      </c>
+      <c r="H67" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>new TableColDef("SID", typeof(String), "objectsid","SID"),</v>
+      </c>
+      <c r="I67" t="str">
+        <f>CONCATENATE("[",C67,"] [",A67,"](",D67,") ",E67,",")</f>
+        <v>[SID] [nvarchar](128) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" t="s">
+        <v>47</v>
+      </c>
+      <c r="E68" t="s">
+        <v>97</v>
+      </c>
+      <c r="F68" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G68" t="s">
         <v>70</v>
       </c>
-      <c r="H67" s="1" t="str">
-        <f t="shared" ref="H67" si="1">CONCATENATE("new TableColDef(""",C67,""", typeof(",B67,"), """,G67,""",""",F67,"""),")</f>
+      <c r="H68" s="1" t="str">
+        <f t="shared" ref="H68" si="3">CONCATENATE("new TableColDef(""",C68,""", typeof(",B68,"), """,G68,""",""",F68,"""),")</f>
         <v>new TableColDef("ObjectGUID", typeof(Guid), "Guid","ObjGuid"),</v>
       </c>
-      <c r="I67" t="str">
-        <f>CONCATENATE("[",C67,"] [",A67,"] ",E67,",")</f>
+      <c r="I68" t="str">
+        <f>CONCATENATE("[",C68,"] [",A68,"] ",E68,",")</f>
         <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
       </c>
     </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>46</v>
+      </c>
+      <c r="B69" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69" t="s">
+        <v>180</v>
+      </c>
+      <c r="E69" t="s">
+        <v>96</v>
+      </c>
+      <c r="G69"/>
+      <c r="H69" t="s">
+        <v>181</v>
+      </c>
+      <c r="I69" t="str">
+        <f>CONCATENATE("[",C69,"] [",A69,"] ",E69,",")</f>
+        <v>[ManagerGUID] [uniqueidentifier] NULL,</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I60"/>
+  <autoFilter ref="A1:I61"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3004,7 +3066,7 @@
         <v>new TableColDef("GivenName", typeof(String), "givenname","Adprop"),</v>
       </c>
       <c r="I2" t="str">
-        <f>CONCATENATE("[",C2,"] [",A2,"](",D2,") ",E2,",")</f>
+        <f t="shared" ref="I2:I30" si="0">CONCATENATE("[",C2,"] [",A2,"](",D2,") ",E2,",")</f>
         <v>[GivenName] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -3031,11 +3093,11 @@
         <v>156</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H35" si="0">CONCATENATE("new TableColDef(""",C3,""", typeof(",B3,"), """,G3,""",""",F3,"""),")</f>
+        <f t="shared" ref="H3:H35" si="1">CONCATENATE("new TableColDef(""",C3,""", typeof(",B3,"), """,G3,""",""",F3,"""),")</f>
         <v>new TableColDef("Initials", typeof(String), "initials","Adprop"),</v>
       </c>
       <c r="I3" t="str">
-        <f>CONCATENATE("[",C3,"] [",A3,"](",D3,") ",E3,",")</f>
+        <f t="shared" si="0"/>
         <v>[Initials] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -3062,11 +3124,11 @@
         <v>103</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Surname", typeof(String), "sn","Adprop"),</v>
       </c>
       <c r="I4" t="str">
-        <f>CONCATENATE("[",C4,"] [",A4,"](",D4,") ",E4,",")</f>
+        <f t="shared" si="0"/>
         <v>[Surname] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -3093,11 +3155,11 @@
         <v>115</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("DisplayName", typeof(String), "displayname","Adprop"),</v>
       </c>
       <c r="I5" t="str">
-        <f>CONCATENATE("[",C5,"] [",A5,"](",D5,") ",E5,",")</f>
+        <f t="shared" si="0"/>
         <v>[DisplayName] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -3124,11 +3186,11 @@
         <v>101</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Description", typeof(String), "description","Adprop"),</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("[",C6,"] [",A6,"](",D6,") ",E6,",")</f>
+        <f t="shared" si="0"/>
         <v>[Description] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -3155,11 +3217,11 @@
         <v>79</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Office", typeof(String), "physicalDeliveryOfficeName","Adprop"),</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE("[",C7,"] [",A7,"](",D7,") ",E7,",")</f>
+        <f t="shared" si="0"/>
         <v>[Office] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -3186,11 +3248,11 @@
         <v>155</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("OfficePhone", typeof(String), "telephonenumber","Adprop"),</v>
       </c>
       <c r="I8" t="str">
-        <f>CONCATENATE("[",C8,"] [",A8,"](",D8,") ",E8,",")</f>
+        <f t="shared" si="0"/>
         <v>[OfficePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -3217,11 +3279,11 @@
         <v>102</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("EmailAddress", typeof(String), "mail","Adprop"),</v>
       </c>
       <c r="I9" t="str">
-        <f>CONCATENATE("[",C9,"] [",A9,"](",D9,") ",E9,",")</f>
+        <f t="shared" si="0"/>
         <v>[EmailAddress] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -3248,11 +3310,11 @@
         <v>165</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("HomePage", typeof(String), "wwwhomepage","Adprop"),</v>
       </c>
       <c r="I10" t="str">
-        <f>CONCATENATE("[",C10,"] [",A10,"](",D10,") ",E10,",")</f>
+        <f t="shared" si="0"/>
         <v>[HomePage] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -3279,11 +3341,11 @@
         <v>171</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("StreetAddress", typeof(String), "streetaddress","Adprop"),</v>
       </c>
       <c r="I11" t="str">
-        <f>CONCATENATE("[",C11,"] [",A11,"](",D11,") ",E11,",")</f>
+        <f t="shared" si="0"/>
         <v>[StreetAddress] [nvarchar](160) NULL,</v>
       </c>
     </row>
@@ -3310,11 +3372,11 @@
         <v>167</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("POBox", typeof(String), "postofficebox","Adprop"),</v>
       </c>
       <c r="I12" t="str">
-        <f>CONCATENATE("[",C12,"] [",A12,"](",D12,") ",E12,",")</f>
+        <f t="shared" si="0"/>
         <v>[POBox] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -3341,11 +3403,11 @@
         <v>83</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("City", typeof(String), "l","Adprop"),</v>
       </c>
       <c r="I13" t="str">
-        <f>CONCATENATE("[",C13,"] [",A13,"](",D13,") ",E13,",")</f>
+        <f t="shared" si="0"/>
         <v>[City] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -3372,11 +3434,11 @@
         <v>78</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("State", typeof(String), "st","Adprop"),</v>
       </c>
       <c r="I14" t="str">
-        <f>CONCATENATE("[",C14,"] [",A14,"](",D14,") ",E14,",")</f>
+        <f t="shared" si="0"/>
         <v>[State] [nvarchar](64) NULL,</v>
       </c>
     </row>
@@ -3403,11 +3465,11 @@
         <v>168</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("PostalCode", typeof(String), "postalcode","Adprop"),</v>
       </c>
       <c r="I15" t="str">
-        <f>CONCATENATE("[",C15,"] [",A15,"](",D15,") ",E15,",")</f>
+        <f t="shared" si="0"/>
         <v>[PostalCode] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -3434,11 +3496,11 @@
         <v>77</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Country", typeof(String), "co","Adprop"),</v>
       </c>
       <c r="I16" t="str">
-        <f>CONCATENATE("[",C16,"] [",A16,"](",D16,") ",E16,",")</f>
+        <f t="shared" si="0"/>
         <v>[Country] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -3465,11 +3527,11 @@
         <v>160</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("HomePhone", typeof(String), "homephone","Adprop"),</v>
       </c>
       <c r="I17" t="str">
-        <f>CONCATENATE("[",C17,"] [",A17,"](",D17,") ",E17,",")</f>
+        <f t="shared" si="0"/>
         <v>[HomePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -3496,11 +3558,11 @@
         <v>166</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Pager", typeof(String), "pager","Adprop"),</v>
       </c>
       <c r="I18" t="str">
-        <f>CONCATENATE("[",C18,"] [",A18,"](",D18,") ",E18,",")</f>
+        <f t="shared" si="0"/>
         <v>[Pager] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -3527,11 +3589,11 @@
         <v>82</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("MobilePhone", typeof(String), "mobile","Adprop"),</v>
       </c>
       <c r="I19" t="str">
-        <f>CONCATENATE("[",C19,"] [",A19,"](",D19,") ",E19,",")</f>
+        <f t="shared" si="0"/>
         <v>[MobilePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -3558,11 +3620,11 @@
         <v>84</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Fax", typeof(String), "facsimileTelephoneNumber","Adprop"),</v>
       </c>
       <c r="I20" t="str">
-        <f>CONCATENATE("[",C20,"] [",A20,"](",D20,") ",E20,",")</f>
+        <f t="shared" si="0"/>
         <v>[Fax] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -3589,11 +3651,11 @@
         <v>149</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Title", typeof(String), "title","Adprop"),</v>
       </c>
       <c r="I21" t="str">
-        <f>CONCATENATE("[",C21,"] [",A21,"](",D21,") ",E21,",")</f>
+        <f t="shared" si="0"/>
         <v>[Title] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -3620,11 +3682,11 @@
         <v>159</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Department", typeof(String), "department","Adprop"),</v>
       </c>
       <c r="I22" t="str">
-        <f>CONCATENATE("[",C22,"] [",A22,"](",D22,") ",E22,",")</f>
+        <f t="shared" si="0"/>
         <v>[Department] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -3651,11 +3713,11 @@
         <v>154</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Company", typeof(String), "company","Adprop"),</v>
       </c>
       <c r="I23" t="str">
-        <f>CONCATENATE("[",C23,"] [",A23,"](",D23,") ",E23,",")</f>
+        <f t="shared" si="0"/>
         <v>[Company] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -3682,11 +3744,11 @@
         <v>158</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Manager", typeof(String), "manager","Adprop"),</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE("[",C24,"] [",A24,"](",D24,") ",E24,",")</f>
+        <f t="shared" si="0"/>
         <v>[Manager] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -3713,11 +3775,11 @@
         <v>152</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("EmployeeID", typeof(String), "employeeid","Adprop"),</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE("[",C25,"] [",A25,"](",D25,") ",E25,",")</f>
+        <f t="shared" si="0"/>
         <v>[EmployeeID] [nvarchar](64) NULL,</v>
       </c>
     </row>
@@ -3744,11 +3806,11 @@
         <v>162</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("EmployeeNumber", typeof(String), "employeenumber","Adprop"),</v>
       </c>
       <c r="I26" t="str">
-        <f>CONCATENATE("[",C26,"] [",A26,"](",D26,") ",E26,",")</f>
+        <f t="shared" si="0"/>
         <v>[EmployeeNumber] [nvarchar](64) NULL,</v>
       </c>
     </row>
@@ -3775,11 +3837,11 @@
         <v>161</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Division", typeof(String), "division","Adprop"),</v>
       </c>
       <c r="I27" t="str">
-        <f>CONCATENATE("[",C27,"] [",A27,"](",D27,") ",E27,",")</f>
+        <f t="shared" si="0"/>
         <v>[Division] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -3806,11 +3868,11 @@
         <v>114</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("DistinguishedName", typeof(String), "distinguishedname","Adprop"),</v>
       </c>
       <c r="I28" t="str">
-        <f>CONCATENATE("[",C28,"] [",A28,"](",D28,") ",E28,",")</f>
+        <f t="shared" si="0"/>
         <v>[DistinguishedName] [nvarchar](512) NULL,</v>
       </c>
     </row>
@@ -3837,11 +3899,11 @@
         <v>104</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Name", typeof(String), "name","Adprop"),</v>
       </c>
       <c r="I29" t="str">
-        <f>CONCATENATE("[",C29,"] [",A29,"](",D29,") ",E29,",")</f>
+        <f t="shared" si="0"/>
         <v>[Name] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -3868,11 +3930,11 @@
         <v>126</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("CN", typeof(String), "cn","Adprop"),</v>
       </c>
       <c r="I30" t="str">
-        <f>CONCATENATE("[",C30,"] [",A30,"](",D30,") ",E30,",")</f>
+        <f t="shared" si="0"/>
         <v>[CN] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -3896,7 +3958,7 @@
         <v>157</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Created", typeof(DateTime), "whencreated","Adprop"),</v>
       </c>
       <c r="I31" t="str">
@@ -3924,7 +3986,7 @@
         <v>151</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Modified", typeof(DateTime), "whenchanged","Adprop"),</v>
       </c>
       <c r="I32" t="str">
@@ -3955,7 +4017,7 @@
         <v>113</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("ObjectCategory", typeof(String), "objectcategory","Adprop"),</v>
       </c>
       <c r="I33" t="str">
@@ -3986,7 +4048,7 @@
         <v>118</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("ObjectClass", typeof(String), "SchemaClassName","ObjClass"),</v>
       </c>
       <c r="I34" t="str">
@@ -4014,7 +4076,7 @@
         <v>70</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("ObjectGUID", typeof(Guid), "Guid","ObjGuid"),</v>
       </c>
       <c r="I35" t="str">
@@ -5357,7 +5419,7 @@
         <v>new TableColDef("Name", typeof(String), "name","Adprop"),</v>
       </c>
       <c r="I2" t="str">
-        <f>CONCATENATE("[",C2,"] [",A2,"](",D2,") ",E2,",")</f>
+        <f t="shared" ref="I2:I9" si="0">CONCATENATE("[",C2,"] [",A2,"](",D2,") ",E2,",")</f>
         <v>[Name] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -5384,11 +5446,11 @@
         <v>117</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H16" si="0">CONCATENATE("new TableColDef(""",C3,""", typeof(",B3,"), """,G3,""",""",F3,"""),")</f>
+        <f t="shared" ref="H3:H16" si="1">CONCATENATE("new TableColDef(""",C3,""", typeof(",B3,"), """,G3,""",""",F3,"""),")</f>
         <v>new TableColDef("GroupCategory", typeof(String), "grouptype","GrpCat"),</v>
       </c>
       <c r="I3" t="str">
-        <f>CONCATENATE("[",C3,"] [",A3,"](",D3,") ",E3,",")</f>
+        <f t="shared" si="0"/>
         <v>[GroupCategory] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -5415,11 +5477,11 @@
         <v>117</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("GroupScope", typeof(String), "grouptype","GrpScope"),</v>
       </c>
       <c r="I4" t="str">
-        <f>CONCATENATE("[",C4,"] [",A4,"](",D4,") ",E4,",")</f>
+        <f t="shared" si="0"/>
         <v>[GroupScope] [nvarchar](32) NULL,</v>
       </c>
     </row>
@@ -5446,11 +5508,11 @@
         <v>101</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Description", typeof(String), "description","Adprop"),</v>
       </c>
       <c r="I5" t="str">
-        <f>CONCATENATE("[",C5,"] [",A5,"](",D5,") ",E5,",")</f>
+        <f t="shared" si="0"/>
         <v>[Description] [nvarchar](512) NULL,</v>
       </c>
     </row>
@@ -5477,11 +5539,11 @@
         <v>102</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("EmailAddress", typeof(String), "mail","Adprop"),</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("[",C6,"] [",A6,"](",D6,") ",E6,",")</f>
+        <f t="shared" si="0"/>
         <v>[EmailAddress] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -5508,11 +5570,11 @@
         <v>116</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("ManagedBy", typeof(String), "managedby","Adprop"),</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE("[",C7,"] [",A7,"](",D7,") ",E7,",")</f>
+        <f t="shared" si="0"/>
         <v>[ManagedBy] [nvarchar](256) NULL,</v>
       </c>
     </row>
@@ -5539,11 +5601,11 @@
         <v>114</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("DistinguishedName", typeof(String), "distinguishedname","Adprop"),</v>
       </c>
       <c r="I8" t="str">
-        <f>CONCATENATE("[",C8,"] [",A8,"](",D8,") ",E8,",")</f>
+        <f t="shared" si="0"/>
         <v>[DistinguishedName] [nvarchar](512) NULL,</v>
       </c>
     </row>
@@ -5570,11 +5632,11 @@
         <v>115</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("DisplayName", typeof(String), "displayname","Adprop"),</v>
       </c>
       <c r="I9" t="str">
-        <f>CONCATENATE("[",C9,"] [",A9,"](",D9,") ",E9,",")</f>
+        <f t="shared" si="0"/>
         <v>[DisplayName] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -5598,7 +5660,7 @@
         <v>80</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Created", typeof(DateTime), "whenCreated","Adprop"),</v>
       </c>
       <c r="I10" t="str">
@@ -5626,7 +5688,7 @@
         <v>81</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("Modified", typeof(DateTime), "whenChanged","Adprop"),</v>
       </c>
       <c r="I11" t="str">
@@ -5657,7 +5719,7 @@
         <v>111</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("SamAccountName", typeof(String), "samaccountname","Adprop"),</v>
       </c>
       <c r="I12" t="str">
@@ -5688,7 +5750,7 @@
         <v>113</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("ObjectCategory", typeof(String), "objectcategory","Adprop"),</v>
       </c>
       <c r="I13" t="str">
@@ -5719,7 +5781,7 @@
         <v>118</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("ObjectClass", typeof(String), "SchemaClassName","ObjClass"),</v>
       </c>
       <c r="I14" t="str">
@@ -5750,11 +5812,11 @@
         <v>112</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("SID", typeof(String), "objectsid","SID"),</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" ref="I15" si="1">CONCATENATE("[",C15,"] [",A15,"](",D15,") ",E15,",")</f>
+        <f t="shared" ref="I15" si="2">CONCATENATE("[",C15,"] [",A15,"](",D15,") ",E15,",")</f>
         <v>[SID] [nvarchar](128) NULL,</v>
       </c>
     </row>
@@ -5778,7 +5840,7 @@
         <v>70</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>new TableColDef("ObjectGUID", typeof(Guid), "Guid","ObjGuid"),</v>
       </c>
       <c r="I16" t="str">

</xml_diff>

<commit_message>
UserMustChangePasswordAtNextLogon column set within the CLR SP
</commit_message>
<xml_diff>
--- a/GetADobjects/AD Column map.xlsx
+++ b/GetADobjects/AD Column map.xlsx
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Computers!$A$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Contacts!$A$1:$I$58</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Groups!$A$1:$I$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Users!$A$1:$I$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Users!$A$1:$I$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WellKnownSIDs!$A$1:$I$8</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="184">
   <si>
     <t>max_length</t>
   </si>
@@ -584,6 +584,9 @@
   </si>
   <si>
     <t>nop</t>
+  </si>
+  <si>
+    <t>UserMustChangePasswordAtNextLogon</t>
   </si>
 </sst>
 </file>
@@ -919,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,7 +1024,7 @@
         <v>156</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H67" si="1">CONCATENATE("new TableColDef(""",C3,""", typeof(",B3,"), """,G3,""",""",F3,"""),")</f>
+        <f t="shared" ref="H3:H68" si="1">CONCATENATE("new TableColDef(""",C3,""", typeof(",B3,"), """,G3,""",""",F3,"""),")</f>
         <v>new TableColDef("Initials", typeof(String), "initials","Adprop"),</v>
       </c>
       <c r="I3" t="str">
@@ -1797,7 +1800,7 @@
         <v>new TableColDef("Enabled", typeof(Boolean), "ACCOUNTDISABLE","UAC"),</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" ref="I28:I50" si="2">CONCATENATE("[",C28,"] [",A28,"] ",E28,",")</f>
+        <f t="shared" ref="I28:I51" si="2">CONCATENATE("[",C28,"] [",A28,"] ",E28,",")</f>
         <v>[Enabled] [bit] NULL,</v>
       </c>
     </row>
@@ -2195,142 +2198,142 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" t="s">
-        <v>35</v>
+        <v>72</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>183</v>
       </c>
       <c r="E43" t="s">
         <v>96</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="G43" t="s">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="H43" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("LastBadPasswordAttempt", typeof(DateTime), "badpasswordtime","filetime"),</v>
+        <v>new TableColDef("UserMustChangePasswordAtNextLogon", typeof(Boolean), "does_not_exist_in_AD","nop"),</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="2"/>
-        <v>[LastBadPasswordAttempt] [datetime] NULL,</v>
+        <v>[UserMustChangePasswordAtNextLogon] [bit] NULL,</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E44" t="s">
         <v>96</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G44" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="H44" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("BadLogonCount", typeof(Int32), "badpwdcount","Adprop"),</v>
+        <v>new TableColDef("LastBadPasswordAttempt", typeof(DateTime), "badpasswordtime","filetime"),</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="2"/>
-        <v>[BadLogonCount] [int] NULL,</v>
+        <v>[LastBadPasswordAttempt] [datetime] NULL,</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C45" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E45" t="s">
         <v>96</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="G45" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="H45" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("LastLogonDate", typeof(DateTime), "lastlogon","filetime"),</v>
+        <v>new TableColDef("BadLogonCount", typeof(Int32), "badpwdcount","Adprop"),</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="2"/>
-        <v>[LastLogonDate] [datetime] NULL,</v>
+        <v>[BadLogonCount] [int] NULL,</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>174</v>
+        <v>73</v>
+      </c>
+      <c r="C46" t="s">
+        <v>36</v>
       </c>
       <c r="E46" t="s">
         <v>96</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G46" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="H46" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("LogonCount", typeof(Int32), "logoncount","Adprop"),</v>
+        <v>new TableColDef("LastLogonDate", typeof(DateTime), "lastlogon","filetime"),</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="2"/>
-        <v>[LogonCount] [int] NULL,</v>
+        <v>[LastLogonDate] [datetime] NULL,</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C47" t="s">
-        <v>51</v>
+        <v>74</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="E47" t="s">
         <v>96</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="G47" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H47" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("PasswordLastSet", typeof(DateTime), "pwdlastset","filetime"),</v>
+        <v>new TableColDef("LogonCount", typeof(Int32), "logoncount","Adprop"),</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="2"/>
-        <v>[PasswordLastSet] [datetime] NULL,</v>
+        <v>[LogonCount] [int] NULL,</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2341,7 +2344,7 @@
         <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="E48" t="s">
         <v>96</v>
@@ -2350,15 +2353,15 @@
         <v>144</v>
       </c>
       <c r="G48" t="s">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="H48" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("PasswordExpiryTime", typeof(DateTime), "msDS-UserPasswordExpiryTimeComputed","filetime"),</v>
+        <v>new TableColDef("PasswordLastSet", typeof(DateTime), "pwdlastset","filetime"),</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="2"/>
-        <v>[PasswordExpiryTime] [datetime] NULL,</v>
+        <v>[PasswordLastSet] [datetime] NULL,</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2369,7 +2372,7 @@
         <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>178</v>
       </c>
       <c r="E49" t="s">
         <v>96</v>
@@ -2378,15 +2381,15 @@
         <v>144</v>
       </c>
       <c r="G49" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="H49" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("AccountLockoutTime", typeof(DateTime), "lockouttime","filetime"),</v>
+        <v>new TableColDef("PasswordExpiryTime", typeof(DateTime), "msDS-UserPasswordExpiryTimeComputed","filetime"),</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="2"/>
-        <v>[AccountLockoutTime] [datetime] NULL,</v>
+        <v>[PasswordExpiryTime] [datetime] NULL,</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2397,7 +2400,7 @@
         <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E50" t="s">
         <v>96</v>
@@ -2406,46 +2409,43 @@
         <v>144</v>
       </c>
       <c r="G50" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="H50" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("AccountExpirationDate", typeof(DateTime), "accountexpires","filetime"),</v>
+        <v>new TableColDef("AccountLockoutTime", typeof(DateTime), "lockouttime","filetime"),</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="2"/>
-        <v>[AccountExpirationDate] [datetime] NULL,</v>
+        <v>[AccountLockoutTime] [datetime] NULL,</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D51">
-        <v>128</v>
+        <v>73</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3</v>
       </c>
       <c r="E51" t="s">
         <v>96</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G51" t="s">
-        <v>172</v>
+        <v>119</v>
       </c>
       <c r="H51" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("LogonWorkstations", typeof(String), "userworkstations","Adprop"),</v>
+        <v>new TableColDef("AccountExpirationDate", typeof(DateTime), "accountexpires","filetime"),</v>
       </c>
       <c r="I51" t="str">
-        <f>CONCATENATE("[",C51,"] [",A51,"](",D51,") ",E51,",")</f>
-        <v>[LogonWorkstations] [nvarchar](128) NULL,</v>
+        <f t="shared" si="2"/>
+        <v>[AccountExpirationDate] [datetime] NULL,</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
         <v>75</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D52">
         <v>128</v>
@@ -2468,15 +2468,15 @@
         <v>147</v>
       </c>
       <c r="G52" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="H52" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("HomeDirectory", typeof(String), "homedirectory","Adprop"),</v>
+        <v>new TableColDef("LogonWorkstations", typeof(String), "userworkstations","Adprop"),</v>
       </c>
       <c r="I52" t="str">
         <f>CONCATENATE("[",C52,"] [",A52,"](",D52,") ",E52,",")</f>
-        <v>[HomeDirectory] [nvarchar](128) NULL,</v>
+        <v>[LogonWorkstations] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2487,10 +2487,10 @@
         <v>75</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D53">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="E53" t="s">
         <v>96</v>
@@ -2499,15 +2499,15 @@
         <v>147</v>
       </c>
       <c r="G53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H53" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("HomeDrive", typeof(String), "homedrive","Adprop"),</v>
+        <v>new TableColDef("HomeDirectory", typeof(String), "homedirectory","Adprop"),</v>
       </c>
       <c r="I53" t="str">
         <f>CONCATENATE("[",C53,"] [",A53,"](",D53,") ",E53,",")</f>
-        <v>[HomeDrive] [nvarchar](64) NULL,</v>
+        <v>[HomeDirectory] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2517,11 +2517,11 @@
       <c r="B54" t="s">
         <v>75</v>
       </c>
-      <c r="C54" t="s">
-        <v>56</v>
+      <c r="C54" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="D54">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="E54" t="s">
         <v>96</v>
@@ -2530,15 +2530,15 @@
         <v>147</v>
       </c>
       <c r="G54" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H54" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("ProfilePath", typeof(String), "profilepath","Adprop"),</v>
+        <v>new TableColDef("HomeDrive", typeof(String), "homedrive","Adprop"),</v>
       </c>
       <c r="I54" t="str">
         <f>CONCATENATE("[",C54,"] [",A54,"](",D54,") ",E54,",")</f>
-        <v>[ProfilePath] [nvarchar](128) NULL,</v>
+        <v>[HomeDrive] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2549,10 +2549,10 @@
         <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D55">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E55" t="s">
         <v>96</v>
@@ -2561,26 +2561,29 @@
         <v>147</v>
       </c>
       <c r="G55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H55" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("ScriptPath", typeof(String), "scriptpath","Adprop"),</v>
+        <v>new TableColDef("ProfilePath", typeof(String), "profilepath","Adprop"),</v>
       </c>
       <c r="I55" t="str">
         <f>CONCATENATE("[",C55,"] [",A55,"](",D55,") ",E55,",")</f>
-        <v>[ScriptPath] [nvarchar](256) NULL,</v>
+        <v>[ProfilePath] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>85</v>
+        <v>58</v>
+      </c>
+      <c r="D56">
+        <v>256</v>
       </c>
       <c r="E56" t="s">
         <v>96</v>
@@ -2589,15 +2592,15 @@
         <v>147</v>
       </c>
       <c r="G56" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="H56" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("userAccountControl", typeof(Int32), "useraccountcontrol","Adprop"),</v>
+        <v>new TableColDef("ScriptPath", typeof(String), "scriptpath","Adprop"),</v>
       </c>
       <c r="I56" t="str">
-        <f>CONCATENATE("[",C56,"] [",A56,"] ",E56,",")</f>
-        <v>[userAccountControl] [int] NULL,</v>
+        <f>CONCATENATE("[",C56,"] [",A56,"](",D56,") ",E56,",")</f>
+        <v>[ScriptPath] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2607,11 +2610,8 @@
       <c r="B57" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D57">
-        <v>128</v>
+      <c r="C57" t="s">
+        <v>85</v>
       </c>
       <c r="E57" t="s">
         <v>96</v>
@@ -2620,29 +2620,29 @@
         <v>147</v>
       </c>
       <c r="G57" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H57" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("PrimaryGroupID", typeof(Int32), "primarygroupid","Adprop"),</v>
+        <v>new TableColDef("userAccountControl", typeof(Int32), "useraccountcontrol","Adprop"),</v>
       </c>
       <c r="I57" t="str">
         <f>CONCATENATE("[",C57,"] [",A57,"] ",E57,",")</f>
-        <v>[PrimaryGroupID] [int] NULL,</v>
+        <v>[userAccountControl] [int] NULL,</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" t="s">
-        <v>43</v>
+        <v>74</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="D58">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E58" t="s">
         <v>96</v>
@@ -2651,15 +2651,15 @@
         <v>147</v>
       </c>
       <c r="G58" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="H58" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("Name", typeof(String), "name","Adprop"),</v>
+        <v>new TableColDef("PrimaryGroupID", typeof(Int32), "primarygroupid","Adprop"),</v>
       </c>
       <c r="I58" t="str">
-        <f>CONCATENATE("[",C58,"] [",A58,"](",D58,") ",E58,",")</f>
-        <v>[Name] [nvarchar](256) NULL,</v>
+        <f>CONCATENATE("[",C58,"] [",A58,"] ",E58,",")</f>
+        <v>[PrimaryGroupID] [int] NULL,</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2670,7 +2670,7 @@
         <v>75</v>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D59">
         <v>256</v>
@@ -2682,15 +2682,15 @@
         <v>147</v>
       </c>
       <c r="G59" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="H59" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("CN", typeof(String), "cn","Adprop"),</v>
+        <v>new TableColDef("Name", typeof(String), "name","Adprop"),</v>
       </c>
       <c r="I59" t="str">
         <f>CONCATENATE("[",C59,"] [",A59,"](",D59,") ",E59,",")</f>
-        <v>[CN] [nvarchar](256) NULL,</v>
+        <v>[Name] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2701,7 +2701,7 @@
         <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="D60">
         <v>256</v>
@@ -2713,15 +2713,15 @@
         <v>147</v>
       </c>
       <c r="G60" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="H60" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("UserPrincipalName", typeof(String), "userprincipalname","Adprop"),</v>
+        <v>new TableColDef("CN", typeof(String), "cn","Adprop"),</v>
       </c>
       <c r="I60" t="str">
         <f>CONCATENATE("[",C60,"] [",A60,"](",D60,") ",E60,",")</f>
-        <v>[UserPrincipalName] [nvarchar](256) NULL,</v>
+        <v>[CN] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2732,10 +2732,10 @@
         <v>75</v>
       </c>
       <c r="C61" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D61">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="E61" t="s">
         <v>96</v>
@@ -2744,15 +2744,15 @@
         <v>147</v>
       </c>
       <c r="G61" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="H61" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("SamAccountName", typeof(String), "samaccountname","Adprop"),</v>
+        <v>new TableColDef("UserPrincipalName", typeof(String), "userprincipalname","Adprop"),</v>
       </c>
       <c r="I61" t="str">
         <f>CONCATENATE("[",C61,"] [",A61,"](",D61,") ",E61,",")</f>
-        <v>[SamAccountName] [nvarchar](128) NULL,</v>
+        <v>[UserPrincipalName] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2763,10 +2763,10 @@
         <v>75</v>
       </c>
       <c r="C62" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="D62">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="E62" t="s">
         <v>96</v>
@@ -2775,26 +2775,29 @@
         <v>147</v>
       </c>
       <c r="G62" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H62" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("DistinguishedName", typeof(String), "distinguishedname","Adprop"),</v>
+        <v>new TableColDef("SamAccountName", typeof(String), "samaccountname","Adprop"),</v>
       </c>
       <c r="I62" t="str">
         <f>CONCATENATE("[",C62,"] [",A62,"](",D62,") ",E62,",")</f>
-        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
+        <v>[SamAccountName] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>16</v>
+        <v>75</v>
+      </c>
+      <c r="C63" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63">
+        <v>512</v>
       </c>
       <c r="E63" t="s">
         <v>96</v>
@@ -2803,15 +2806,15 @@
         <v>147</v>
       </c>
       <c r="G63" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="H63" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("Created", typeof(DateTime), "whencreated","Adprop"),</v>
+        <v>new TableColDef("DistinguishedName", typeof(String), "distinguishedname","Adprop"),</v>
       </c>
       <c r="I63" t="str">
-        <f>CONCATENATE("[",C63,"] [",A63,"] ",E63,",")</f>
-        <v>[Created] [datetime] NULL,</v>
+        <f>CONCATENATE("[",C63,"] [",A63,"](",D63,") ",E63,",")</f>
+        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2822,7 +2825,7 @@
         <v>73</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="E64" t="s">
         <v>96</v>
@@ -2831,29 +2834,26 @@
         <v>147</v>
       </c>
       <c r="G64" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H64" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("Modified", typeof(DateTime), "whenchanged","Adprop"),</v>
+        <v>new TableColDef("Created", typeof(DateTime), "whencreated","Adprop"),</v>
       </c>
       <c r="I64" t="str">
         <f>CONCATENATE("[",C64,"] [",A64,"] ",E64,",")</f>
-        <v>[Modified] [datetime] NULL,</v>
+        <v>[Created] [datetime] NULL,</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" t="s">
-        <v>44</v>
-      </c>
-      <c r="D65">
-        <v>128</v>
+        <v>73</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="E65" t="s">
         <v>96</v>
@@ -2862,15 +2862,15 @@
         <v>147</v>
       </c>
       <c r="G65" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="H65" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("ObjectCategory", typeof(String), "objectcategory","Adprop"),</v>
+        <v>new TableColDef("Modified", typeof(DateTime), "whenchanged","Adprop"),</v>
       </c>
       <c r="I65" t="str">
-        <f>CONCATENATE("[",C65,"] [",A65,"](",D65,") ",E65,",")</f>
-        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
+        <f>CONCATENATE("[",C65,"] [",A65,"] ",E65,",")</f>
+        <v>[Modified] [datetime] NULL,</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2881,27 +2881,27 @@
         <v>75</v>
       </c>
       <c r="C66" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D66">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="E66" t="s">
         <v>96</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G66" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H66" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("ObjectClass", typeof(String), "SchemaClassName","ObjClass"),</v>
+        <v>new TableColDef("ObjectCategory", typeof(String), "objectcategory","Adprop"),</v>
       </c>
       <c r="I66" t="str">
         <f>CONCATENATE("[",C66,"] [",A66,"](",D66,") ",E66,",")</f>
-        <v>[ObjectClass] [nvarchar](64) NULL,</v>
+        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2912,55 +2912,58 @@
         <v>75</v>
       </c>
       <c r="C67" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D67">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="E67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>59</v>
+        <v>145</v>
       </c>
       <c r="G67" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H67" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("SID", typeof(String), "objectsid","SID"),</v>
+        <v>new TableColDef("ObjectClass", typeof(String), "SchemaClassName","ObjClass"),</v>
       </c>
       <c r="I67" t="str">
         <f>CONCATENATE("[",C67,"] [",A67,"](",D67,") ",E67,",")</f>
-        <v>[SID] [nvarchar](128) NOT NULL,</v>
+        <v>[ObjectClass] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C68" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="D68">
+        <v>128</v>
       </c>
       <c r="E68" t="s">
         <v>97</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>146</v>
+        <v>59</v>
       </c>
       <c r="G68" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f t="shared" ref="H68:H69" si="3">CONCATENATE("new TableColDef(""",C68,""", typeof(",B68,"), """,G68,""",""",F68,"""),")</f>
-        <v>new TableColDef("ObjectGUID", typeof(Guid), "Guid","ObjGuid"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("SID", typeof(String), "objectsid","SID"),</v>
       </c>
       <c r="I68" t="str">
-        <f>CONCATENATE("[",C68,"] [",A68,"] ",E68,",")</f>
-        <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
+        <f>CONCATENATE("[",C68,"] [",A68,"](",D68,") ",E68,",")</f>
+        <v>[SID] [nvarchar](128) NOT NULL,</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2971,28 +2974,56 @@
         <v>70</v>
       </c>
       <c r="C69" t="s">
+        <v>47</v>
+      </c>
+      <c r="E69" t="s">
+        <v>97</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G69" t="s">
+        <v>70</v>
+      </c>
+      <c r="H69" s="1" t="str">
+        <f t="shared" ref="H69:H70" si="3">CONCATENATE("new TableColDef(""",C69,""", typeof(",B69,"), """,G69,""",""",F69,"""),")</f>
+        <v>new TableColDef("ObjectGUID", typeof(Guid), "Guid","ObjGuid"),</v>
+      </c>
+      <c r="I69" t="str">
+        <f>CONCATENATE("[",C69,"] [",A69,"] ",E69,",")</f>
+        <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" t="s">
         <v>180</v>
       </c>
-      <c r="E69" t="s">
-        <v>96</v>
-      </c>
-      <c r="F69" s="5" t="s">
+      <c r="E70" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G70" t="s">
         <v>181</v>
       </c>
-      <c r="H69" s="1" t="str">
+      <c r="H70" s="1" t="str">
         <f t="shared" si="3"/>
         <v>new TableColDef("ManagerGUID", typeof(Guid), "does_not_exist_in_AD","nop"),</v>
       </c>
-      <c r="I69" t="str">
-        <f>CONCATENATE("[",C69,"] [",A69,"] ",E69,",")</f>
+      <c r="I70" t="str">
+        <f>CONCATENATE("[",C70,"] [",A70,"] ",E70,",")</f>
         <v>[ManagerGUID] [uniqueidentifier] NULL,</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I61"/>
+  <autoFilter ref="A1:I70"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>